<commit_message>
Last Change i hope
</commit_message>
<xml_diff>
--- a/DocsAgenda/Lab3/Lab03_WBT_TCs_Form.xlsx
+++ b/DocsAgenda/Lab3/Lab03_WBT_TCs_Form.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Statement" sheetId="1" state="visible" r:id="rId2"/>
@@ -109,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="123">
   <si>
     <t xml:space="preserve">do not print this form</t>
   </si>
@@ -328,6 +328,9 @@
   </si>
   <si>
     <t xml:space="preserve">1,2,6,7,8,10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not possible</t>
   </si>
   <si>
     <t xml:space="preserve">F02_Cond1:=</t>
@@ -1453,9 +1456,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>732960</xdr:colOff>
+      <xdr:colOff>732240</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>19440</xdr:rowOff>
+      <xdr:rowOff>18720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1469,7 +1472,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="533520" y="1209600"/>
-          <a:ext cx="5025240" cy="3515040"/>
+          <a:ext cx="5021280" cy="3514320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1490,9 +1493,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>746280</xdr:colOff>
+      <xdr:colOff>745560</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>47160</xdr:rowOff>
+      <xdr:rowOff>46440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1505,8 +1508,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6401160" y="1598400"/>
-          <a:ext cx="5229000" cy="4420800"/>
+          <a:off x="6396480" y="1598400"/>
+          <a:ext cx="5225040" cy="4420080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1530,7 +1533,7 @@
   <dimension ref="A1:Z12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4664,8 +4667,8 @@
   </sheetPr>
   <dimension ref="A1:AB20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="U23" activeCellId="0" sqref="U23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5252,7 +5255,9 @@
         <v>62</v>
       </c>
       <c r="R13" s="38"/>
-      <c r="S13" s="38"/>
+      <c r="S13" s="38" t="s">
+        <v>62</v>
+      </c>
       <c r="T13" s="38"/>
       <c r="U13" s="38"/>
       <c r="V13" s="39"/>
@@ -5330,12 +5335,16 @@
       <c r="M15" s="37"/>
       <c r="N15" s="37"/>
       <c r="O15" s="37"/>
-      <c r="P15" s="38"/>
+      <c r="P15" s="38" t="s">
+        <v>73</v>
+      </c>
       <c r="Q15" s="38"/>
       <c r="R15" s="38"/>
       <c r="S15" s="38"/>
       <c r="T15" s="38"/>
-      <c r="U15" s="38"/>
+      <c r="U15" s="38" t="s">
+        <v>73</v>
+      </c>
       <c r="V15" s="39"/>
       <c r="W15" s="39"/>
       <c r="X15" s="39"/>
@@ -5377,10 +5386,10 @@
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -5411,10 +5420,10 @@
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="1"/>
       <c r="B18" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C18" s="43" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -5445,10 +5454,10 @@
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="1"/>
       <c r="B19" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -6508,8 +6517,8 @@
   </sheetPr>
   <dimension ref="A1:Z18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K24" activeCellId="0" sqref="K24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6594,7 +6603,7 @@
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
       <c r="B3" s="44" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C3" s="44"/>
       <c r="D3" s="44"/>
@@ -6624,16 +6633,16 @@
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1"/>
       <c r="B4" s="45" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C4" s="46" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D4" s="47" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E4" s="48" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F4" s="48"/>
       <c r="G4" s="48"/>
@@ -6641,7 +6650,7 @@
       <c r="I4" s="48"/>
       <c r="J4" s="48"/>
       <c r="K4" s="48" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L4" s="48"/>
       <c r="M4" s="1"/>
@@ -6665,26 +6674,26 @@
       <c r="C5" s="46"/>
       <c r="D5" s="47"/>
       <c r="E5" s="49" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F5" s="49" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G5" s="49" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H5" s="49" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I5" s="49" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="J5" s="49"/>
       <c r="K5" s="49" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="L5" s="49" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
@@ -6707,25 +6716,25 @@
         <v>9</v>
       </c>
       <c r="C6" s="50" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D6" s="51" t="s">
         <v>59</v>
       </c>
       <c r="E6" s="52" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F6" s="52" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G6" s="52" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H6" s="52" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I6" s="52" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J6" s="52"/>
       <c r="K6" s="52" t="n">
@@ -6758,22 +6767,22 @@
       </c>
       <c r="C7" s="50"/>
       <c r="D7" s="51" t="s">
+        <v>97</v>
+      </c>
+      <c r="E7" s="48" t="s">
+        <v>94</v>
+      </c>
+      <c r="F7" s="48" t="s">
+        <v>95</v>
+      </c>
+      <c r="G7" s="52" t="s">
+        <v>95</v>
+      </c>
+      <c r="H7" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="I7" s="48" t="s">
         <v>96</v>
-      </c>
-      <c r="E7" s="48" t="s">
-        <v>93</v>
-      </c>
-      <c r="F7" s="48" t="s">
-        <v>94</v>
-      </c>
-      <c r="G7" s="52" t="s">
-        <v>94</v>
-      </c>
-      <c r="H7" s="48" t="s">
-        <v>88</v>
-      </c>
-      <c r="I7" s="48" t="s">
-        <v>95</v>
       </c>
       <c r="J7" s="48"/>
       <c r="K7" s="48" t="n">
@@ -6806,22 +6815,22 @@
       </c>
       <c r="C8" s="50"/>
       <c r="D8" s="53" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E8" s="48" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F8" s="48" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G8" s="48" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H8" s="48" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I8" s="48" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J8" s="48"/>
       <c r="K8" s="48" t="n">
@@ -6854,22 +6863,22 @@
       </c>
       <c r="C9" s="50"/>
       <c r="D9" s="53" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E9" s="48" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F9" s="48" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="G9" s="48" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H9" s="48" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I9" s="48" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J9" s="48"/>
       <c r="K9" s="48" t="n">
@@ -6902,22 +6911,22 @@
       </c>
       <c r="C10" s="50"/>
       <c r="D10" s="54" t="s">
+        <v>106</v>
+      </c>
+      <c r="E10" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="F10" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="G10" s="48" t="s">
         <v>105</v>
       </c>
-      <c r="E10" s="49" t="s">
-        <v>98</v>
-      </c>
-      <c r="F10" s="48" t="s">
-        <v>103</v>
-      </c>
-      <c r="G10" s="48" t="s">
-        <v>104</v>
-      </c>
       <c r="H10" s="48" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I10" s="49" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J10" s="49"/>
       <c r="K10" s="49" t="n">
@@ -7002,7 +7011,7 @@
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="1"/>
       <c r="B13" s="55" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -7033,24 +7042,24 @@
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="58" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D14" s="58"/>
       <c r="E14" s="58"/>
       <c r="F14" s="58"/>
       <c r="G14" s="58"/>
       <c r="H14" s="59" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="I14" s="58" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="J14" s="58"/>
       <c r="K14" s="58"/>
       <c r="L14" s="58"/>
       <c r="M14" s="58"/>
       <c r="N14" s="60" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="O14" s="60"/>
       <c r="P14" s="1"/>
@@ -7068,46 +7077,46 @@
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="1"/>
       <c r="B15" s="61" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C15" s="62" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D15" s="63" t="s">
+        <v>113</v>
+      </c>
+      <c r="E15" s="63" t="s">
+        <v>114</v>
+      </c>
+      <c r="F15" s="64" t="s">
+        <v>115</v>
+      </c>
+      <c r="G15" s="65" t="s">
+        <v>116</v>
+      </c>
+      <c r="H15" s="66" t="s">
+        <v>117</v>
+      </c>
+      <c r="I15" s="67" t="s">
+        <v>118</v>
+      </c>
+      <c r="J15" s="63" t="s">
         <v>112</v>
       </c>
-      <c r="E15" s="63" t="s">
+      <c r="K15" s="63" t="s">
         <v>113</v>
       </c>
-      <c r="F15" s="64" t="s">
-        <v>114</v>
-      </c>
-      <c r="G15" s="65" t="s">
+      <c r="L15" s="68" t="s">
+        <v>119</v>
+      </c>
+      <c r="M15" s="69" t="s">
         <v>115</v>
       </c>
-      <c r="H15" s="66" t="s">
-        <v>116</v>
-      </c>
-      <c r="I15" s="67" t="s">
-        <v>117</v>
-      </c>
-      <c r="J15" s="63" t="s">
-        <v>111</v>
-      </c>
-      <c r="K15" s="63" t="s">
-        <v>112</v>
-      </c>
-      <c r="L15" s="68" t="s">
+      <c r="N15" s="70" t="s">
         <v>118</v>
       </c>
-      <c r="M15" s="69" t="s">
-        <v>114</v>
-      </c>
-      <c r="N15" s="70" t="s">
-        <v>117</v>
-      </c>
       <c r="O15" s="71" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
@@ -7152,7 +7161,7 @@
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="1"/>
       <c r="B17" s="72" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C17" s="62" t="n">
         <v>5</v>
@@ -7162,14 +7171,14 @@
       </c>
       <c r="E17" s="73"/>
       <c r="F17" s="74" t="n">
-        <v>66</v>
+        <v>0</v>
       </c>
       <c r="G17" s="75"/>
       <c r="H17" s="76" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="I17" s="77" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="J17" s="78" t="n">
         <f aca="false">SUM(K17:L17)</f>
@@ -7179,7 +7188,7 @@
       <c r="L17" s="79"/>
       <c r="M17" s="80"/>
       <c r="N17" s="81" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="O17" s="82" t="n">
         <f aca="false">D17</f>

</xml_diff>